<commit_message>
feat: support save as bytes.Buffer, delete default sheet, add setNoDataSheetHeaders
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,7 +7,8 @@
     <workbookView windowHeight="8010" windowWidth="14805" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="用户信息" sheetId="2" relationships:id="rId4"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="2" relationships:id="rId4"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet2" sheetId="3" relationships:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -321,47 +322,330 @@
 <worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>string</v>
+      </c>
+      <c r="B1" t="str">
+        <v>int</v>
+      </c>
+      <c r="C1" t="str">
+        <v>float</v>
+      </c>
+      <c r="D1" t="str">
+        <v>bool</v>
+      </c>
+      <c r="E1" t="str">
+        <v>time</v>
+      </c>
+      <c r="F1" t="str">
+        <v>string pointer</v>
+      </c>
+      <c r="G1" t="str">
+        <v>int pointer</v>
+      </c>
+      <c r="H1" t="str">
+        <v>float pointer</v>
+      </c>
+      <c r="I1" t="str">
+        <v>bool pointer</v>
+      </c>
+      <c r="J1" t="str">
+        <v>time pointer</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>string</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <v>1.10e+00</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F2" t="str"/>
+      <c r="G2" t="str"/>
+      <c r="H2" t="str"/>
+      <c r="I2" t="str"/>
+      <c r="J2" t="str"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>string</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v>1.10e+00</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F3" t="str"/>
+      <c r="G3" t="str"/>
+      <c r="H3" t="str"/>
+      <c r="I3" t="str"/>
+      <c r="J3" t="str"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>string</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <v>1.10e+00</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F4" t="str"/>
+      <c r="G4" t="str"/>
+      <c r="H4" t="str"/>
+      <c r="I4" t="str"/>
+      <c r="J4" t="str"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>string</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <v>1.10e+00</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F5" t="str"/>
+      <c r="G5" t="str"/>
+      <c r="H5" t="str"/>
+      <c r="I5" t="str"/>
+      <c r="J5" t="str"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>string</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <v>1.10e+00</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F6" t="str"/>
+      <c r="G6" t="str"/>
+      <c r="H6" t="str"/>
+      <c r="I6" t="str"/>
+      <c r="J6" t="str"/>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>姓名</v>
+        <v>string</v>
       </c>
       <c r="B1" t="str">
-        <v>年龄</v>
+        <v>int</v>
       </c>
       <c r="C1" t="str">
-        <v>生日</v>
+        <v>float</v>
       </c>
       <c r="D1" t="str">
-        <v>工作</v>
+        <v>bool</v>
+      </c>
+      <c r="E1" t="str">
+        <v>time</v>
+      </c>
+      <c r="F1" t="str">
+        <v>string pointer</v>
+      </c>
+      <c r="G1" t="str">
+        <v>int pointer</v>
+      </c>
+      <c r="H1" t="str">
+        <v>float pointer</v>
+      </c>
+      <c r="I1" t="str">
+        <v>bool pointer</v>
+      </c>
+      <c r="J1" t="str">
+        <v>time pointer</v>
+      </c>
+      <c r="K1" t="str">
+        <v>float32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>张三</v>
+        <v>string</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C2" t="str">
-        <v>2024-01-21 16:49:52</v>
-      </c>
-      <c r="D2" t="str"/>
+        <v>1.10e+00</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F2" t="str">
+        <v>string_value</v>
+      </c>
+      <c r="G2" t="str"/>
+      <c r="H2" t="str"/>
+      <c r="I2" t="str"/>
+      <c r="J2" t="str"/>
+      <c r="K2" t="str">
+        <v>0.00e+00</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>李四</v>
+        <v>string</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C3" t="str">
-        <v>2024-01-21 16:49:52</v>
-      </c>
-      <c r="D3" t="str">
-        <v>程序员</v>
+        <v>1.10e+00</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F3" t="str">
+        <v>string_value</v>
+      </c>
+      <c r="G3" t="str"/>
+      <c r="H3" t="str"/>
+      <c r="I3" t="str"/>
+      <c r="J3" t="str"/>
+      <c r="K3" t="str">
+        <v>0.00e+00</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>string</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <v>1.10e+00</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F4" t="str">
+        <v>string_value</v>
+      </c>
+      <c r="G4" t="str"/>
+      <c r="H4" t="str"/>
+      <c r="I4" t="str"/>
+      <c r="J4" t="str"/>
+      <c r="K4" t="str">
+        <v>0.00e+00</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>string</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <v>1.10e+00</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F5" t="str">
+        <v>string_value</v>
+      </c>
+      <c r="G5" t="str"/>
+      <c r="H5" t="str"/>
+      <c r="I5" t="str"/>
+      <c r="J5" t="str"/>
+      <c r="K5" t="str">
+        <v>0.00e+00</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>string</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <v>1.10e+00</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <v>2024-01-24 18:57:32</v>
+      </c>
+      <c r="F6" t="str">
+        <v>string_value</v>
+      </c>
+      <c r="G6" t="str"/>
+      <c r="H6" t="str"/>
+      <c r="I6" t="str"/>
+      <c r="J6" t="str"/>
+      <c r="K6" t="str">
+        <v>0.00e+00</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add fileName validation
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -371,7 +371,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F2" t="str"/>
       <c r="G2" t="str"/>
@@ -393,7 +393,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F3" t="str"/>
       <c r="G3" t="str"/>
@@ -415,7 +415,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F4" t="str"/>
       <c r="G4" t="str"/>
@@ -437,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F5" t="str"/>
       <c r="G5" t="str"/>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F6" t="str"/>
       <c r="G6" t="str"/>
@@ -527,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F2" t="str">
         <v>string_value</v>
@@ -554,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F3" t="str">
         <v>string_value</v>
@@ -581,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F4" t="str">
         <v>string_value</v>
@@ -608,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F5" t="str">
         <v>string_value</v>
@@ -635,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="str">
-        <v>2024-01-24 18:57:32</v>
+        <v>2024-01-24 19:01:27</v>
       </c>
       <c r="F6" t="str">
         <v>string_value</v>

</xml_diff>